<commit_message>
[update] : Player Stat 레벨링 저장 /불러오기 구현
</commit_message>
<xml_diff>
--- a/Assets/Resources/ExcelDB/StageDB.xlsx
+++ b/Assets/Resources/ExcelDB/StageDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\IdleSoul\Assets\Resources\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEBE027-76AF-4846-9950-FA941018FC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3DD11A-BBCC-467E-B109-AF57121399BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F213A0E4-2BEB-43C5-AC4B-881D0214E9F5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -76,18 +76,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>StageMapPath</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefabs/Stage/CasthleStageMap</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>SummonEnemyIDList</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -114,6 +102,21 @@
   <si>
     <t>50005002</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enum&lt;Sizes&gt;</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>StageName</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Casthle</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forest</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1106,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1139,16 +1142,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1180,7 +1183,7 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1206,13 +1209,13 @@
         <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1235,7 +1238,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H4" s="1">
         <v>5500</v>
@@ -1244,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1267,7 +1270,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H5" s="1">
         <v>5500</v>
@@ -1276,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1299,7 +1302,7 @@
         <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H6" s="1">
         <v>5500</v>
@@ -1308,7 +1311,7 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1331,7 +1334,7 @@
         <v>50</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1">
         <v>5500</v>
@@ -1340,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1363,7 +1366,7 @@
         <v>100</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H8" s="1">
         <v>5500</v>
@@ -1372,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1395,7 +1398,7 @@
         <v>120</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H9" s="1">
         <v>5501</v>
@@ -1404,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1427,7 +1430,7 @@
         <v>100</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H10" s="1">
         <v>5501</v>
@@ -1436,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1459,7 +1462,7 @@
         <v>120</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H11" s="1">
         <v>5501</v>
@@ -1468,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1491,7 +1494,7 @@
         <v>100</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H12" s="1">
         <v>5501</v>
@@ -1500,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1523,7 +1526,7 @@
         <v>120</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H13" s="1">
         <v>5501</v>
@@ -1532,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>